<commit_message>
major updates - final figure v6.2
</commit_message>
<xml_diff>
--- a/data/nosulfate/NO_SUL_INFO.xlsx
+++ b/data/nosulfate/NO_SUL_INFO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/sbp29_pitt_edu/Documents/Carvunis Lab/Methionine Project/No Sulfate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SBP29/Desktop/Methionine/NoSulfate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B1DE0E9D-B6BA-8444-BADB-2D29DE7D9C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63F0BFC6-1590-3649-8763-7C2C10761B01}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9DDE23-FC86-5D4E-9442-62B4A681BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{45B8E0A8-28EE-2C48-8E8B-6BF68FC14E1D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{45B8E0A8-28EE-2C48-8E8B-6BF68FC14E1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="49">
   <si>
     <t>batch</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>MM_GAL_R3</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>SD+Met+Glu_Agar</t>
+  </si>
+  <si>
+    <t>Re1</t>
+  </si>
+  <si>
+    <t>AWAY_PM_AGAR_R2</t>
   </si>
 </sst>
 </file>
@@ -524,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56031E3-94A5-8249-ACAE-88A52381765D}">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:H269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:A191"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5603,6 +5618,2034 @@
         <v>12</v>
       </c>
     </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>336</v>
+      </c>
+      <c r="B192" t="s">
+        <v>22</v>
+      </c>
+      <c r="C192" t="s">
+        <v>44</v>
+      </c>
+      <c r="D192">
+        <v>41</v>
+      </c>
+      <c r="E192" t="s">
+        <v>14</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G192">
+        <v>384</v>
+      </c>
+      <c r="H192" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>336</v>
+      </c>
+      <c r="B193" t="s">
+        <v>22</v>
+      </c>
+      <c r="C193" t="s">
+        <v>44</v>
+      </c>
+      <c r="D193">
+        <v>42</v>
+      </c>
+      <c r="E193" t="s">
+        <v>18</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G193">
+        <v>384</v>
+      </c>
+      <c r="H193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>336</v>
+      </c>
+      <c r="B194" t="s">
+        <v>22</v>
+      </c>
+      <c r="C194" t="s">
+        <v>44</v>
+      </c>
+      <c r="D194">
+        <v>43</v>
+      </c>
+      <c r="E194" t="s">
+        <v>19</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G194">
+        <v>384</v>
+      </c>
+      <c r="H194" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>336</v>
+      </c>
+      <c r="B195" t="s">
+        <v>22</v>
+      </c>
+      <c r="C195" t="s">
+        <v>44</v>
+      </c>
+      <c r="D195">
+        <v>44</v>
+      </c>
+      <c r="E195" t="s">
+        <v>14</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G195">
+        <v>384</v>
+      </c>
+      <c r="H195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>336</v>
+      </c>
+      <c r="B196" t="s">
+        <v>22</v>
+      </c>
+      <c r="C196" t="s">
+        <v>44</v>
+      </c>
+      <c r="D196">
+        <v>45</v>
+      </c>
+      <c r="E196" t="s">
+        <v>18</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G196">
+        <v>384</v>
+      </c>
+      <c r="H196" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>336</v>
+      </c>
+      <c r="B197" t="s">
+        <v>22</v>
+      </c>
+      <c r="C197" t="s">
+        <v>44</v>
+      </c>
+      <c r="D197">
+        <v>46</v>
+      </c>
+      <c r="E197" t="s">
+        <v>19</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G197">
+        <v>384</v>
+      </c>
+      <c r="H197" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>336</v>
+      </c>
+      <c r="B198" t="s">
+        <v>22</v>
+      </c>
+      <c r="C198" t="s">
+        <v>44</v>
+      </c>
+      <c r="D198">
+        <v>47</v>
+      </c>
+      <c r="E198" t="s">
+        <v>14</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G198">
+        <v>384</v>
+      </c>
+      <c r="H198" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>336</v>
+      </c>
+      <c r="B199" t="s">
+        <v>22</v>
+      </c>
+      <c r="C199" t="s">
+        <v>44</v>
+      </c>
+      <c r="D199">
+        <v>48</v>
+      </c>
+      <c r="E199" t="s">
+        <v>18</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G199">
+        <v>384</v>
+      </c>
+      <c r="H199" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>336</v>
+      </c>
+      <c r="B200" t="s">
+        <v>22</v>
+      </c>
+      <c r="C200" t="s">
+        <v>44</v>
+      </c>
+      <c r="D200">
+        <v>49</v>
+      </c>
+      <c r="E200" t="s">
+        <v>19</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G200">
+        <v>384</v>
+      </c>
+      <c r="H200" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>336</v>
+      </c>
+      <c r="B201" t="s">
+        <v>22</v>
+      </c>
+      <c r="C201" t="s">
+        <v>44</v>
+      </c>
+      <c r="D201">
+        <v>50</v>
+      </c>
+      <c r="E201" t="s">
+        <v>14</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G201">
+        <v>384</v>
+      </c>
+      <c r="H201" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>336</v>
+      </c>
+      <c r="B202" t="s">
+        <v>22</v>
+      </c>
+      <c r="C202" t="s">
+        <v>44</v>
+      </c>
+      <c r="D202">
+        <v>51</v>
+      </c>
+      <c r="E202" t="s">
+        <v>18</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G202">
+        <v>384</v>
+      </c>
+      <c r="H202" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>336</v>
+      </c>
+      <c r="B203" t="s">
+        <v>22</v>
+      </c>
+      <c r="C203" t="s">
+        <v>44</v>
+      </c>
+      <c r="D203">
+        <v>52</v>
+      </c>
+      <c r="E203" t="s">
+        <v>19</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G203">
+        <v>384</v>
+      </c>
+      <c r="H203" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>336</v>
+      </c>
+      <c r="B204" t="s">
+        <v>22</v>
+      </c>
+      <c r="C204" t="s">
+        <v>44</v>
+      </c>
+      <c r="D204">
+        <v>53</v>
+      </c>
+      <c r="E204" t="s">
+        <v>14</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G204">
+        <v>384</v>
+      </c>
+      <c r="H204" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>336</v>
+      </c>
+      <c r="B205" t="s">
+        <v>22</v>
+      </c>
+      <c r="C205" t="s">
+        <v>44</v>
+      </c>
+      <c r="D205">
+        <v>54</v>
+      </c>
+      <c r="E205" t="s">
+        <v>18</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G205">
+        <v>384</v>
+      </c>
+      <c r="H205" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>336</v>
+      </c>
+      <c r="B206" t="s">
+        <v>22</v>
+      </c>
+      <c r="C206" t="s">
+        <v>44</v>
+      </c>
+      <c r="D206">
+        <v>55</v>
+      </c>
+      <c r="E206" t="s">
+        <v>19</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G206">
+        <v>384</v>
+      </c>
+      <c r="H206" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>336</v>
+      </c>
+      <c r="B207" t="s">
+        <v>22</v>
+      </c>
+      <c r="C207" t="s">
+        <v>44</v>
+      </c>
+      <c r="D207">
+        <v>56</v>
+      </c>
+      <c r="E207" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G207">
+        <v>384</v>
+      </c>
+      <c r="H207" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>336</v>
+      </c>
+      <c r="B208" t="s">
+        <v>22</v>
+      </c>
+      <c r="C208" t="s">
+        <v>44</v>
+      </c>
+      <c r="D208">
+        <v>57</v>
+      </c>
+      <c r="E208" t="s">
+        <v>18</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G208">
+        <v>384</v>
+      </c>
+      <c r="H208" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>336</v>
+      </c>
+      <c r="B209" t="s">
+        <v>22</v>
+      </c>
+      <c r="C209" t="s">
+        <v>44</v>
+      </c>
+      <c r="D209">
+        <v>58</v>
+      </c>
+      <c r="E209" t="s">
+        <v>19</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G209">
+        <v>384</v>
+      </c>
+      <c r="H209" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>336</v>
+      </c>
+      <c r="B210" t="s">
+        <v>22</v>
+      </c>
+      <c r="C210" t="s">
+        <v>44</v>
+      </c>
+      <c r="D210">
+        <v>59</v>
+      </c>
+      <c r="E210" t="s">
+        <v>14</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G210">
+        <v>384</v>
+      </c>
+      <c r="H210" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>336</v>
+      </c>
+      <c r="B211" t="s">
+        <v>22</v>
+      </c>
+      <c r="C211" t="s">
+        <v>44</v>
+      </c>
+      <c r="D211">
+        <v>60</v>
+      </c>
+      <c r="E211" t="s">
+        <v>18</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G211">
+        <v>384</v>
+      </c>
+      <c r="H211" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>336</v>
+      </c>
+      <c r="B212" t="s">
+        <v>22</v>
+      </c>
+      <c r="C212" t="s">
+        <v>44</v>
+      </c>
+      <c r="D212">
+        <v>61</v>
+      </c>
+      <c r="E212" t="s">
+        <v>19</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G212">
+        <v>384</v>
+      </c>
+      <c r="H212" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>336</v>
+      </c>
+      <c r="B213" t="s">
+        <v>22</v>
+      </c>
+      <c r="C213" t="s">
+        <v>44</v>
+      </c>
+      <c r="D213">
+        <v>62</v>
+      </c>
+      <c r="E213" t="s">
+        <v>14</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G213">
+        <v>384</v>
+      </c>
+      <c r="H213" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>336</v>
+      </c>
+      <c r="B214" t="s">
+        <v>22</v>
+      </c>
+      <c r="C214" t="s">
+        <v>44</v>
+      </c>
+      <c r="D214">
+        <v>63</v>
+      </c>
+      <c r="E214" t="s">
+        <v>18</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G214">
+        <v>384</v>
+      </c>
+      <c r="H214" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>336</v>
+      </c>
+      <c r="B215" t="s">
+        <v>22</v>
+      </c>
+      <c r="C215" t="s">
+        <v>44</v>
+      </c>
+      <c r="D215">
+        <v>64</v>
+      </c>
+      <c r="E215" t="s">
+        <v>19</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G215">
+        <v>384</v>
+      </c>
+      <c r="H215" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>336</v>
+      </c>
+      <c r="B216" t="s">
+        <v>22</v>
+      </c>
+      <c r="C216" t="s">
+        <v>44</v>
+      </c>
+      <c r="D216">
+        <v>65</v>
+      </c>
+      <c r="E216" t="s">
+        <v>14</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G216">
+        <v>384</v>
+      </c>
+      <c r="H216" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>336</v>
+      </c>
+      <c r="B217" t="s">
+        <v>22</v>
+      </c>
+      <c r="C217" t="s">
+        <v>44</v>
+      </c>
+      <c r="D217">
+        <v>66</v>
+      </c>
+      <c r="E217" t="s">
+        <v>18</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G217">
+        <v>384</v>
+      </c>
+      <c r="H217" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>336</v>
+      </c>
+      <c r="B218" t="s">
+        <v>22</v>
+      </c>
+      <c r="C218" t="s">
+        <v>44</v>
+      </c>
+      <c r="D218">
+        <v>67</v>
+      </c>
+      <c r="E218" t="s">
+        <v>19</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G218">
+        <v>384</v>
+      </c>
+      <c r="H218" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>336</v>
+      </c>
+      <c r="B219" t="s">
+        <v>22</v>
+      </c>
+      <c r="C219" t="s">
+        <v>44</v>
+      </c>
+      <c r="D219">
+        <v>68</v>
+      </c>
+      <c r="E219" t="s">
+        <v>14</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G219">
+        <v>384</v>
+      </c>
+      <c r="H219" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>336</v>
+      </c>
+      <c r="B220" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" t="s">
+        <v>44</v>
+      </c>
+      <c r="D220">
+        <v>69</v>
+      </c>
+      <c r="E220" t="s">
+        <v>18</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G220">
+        <v>384</v>
+      </c>
+      <c r="H220" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>336</v>
+      </c>
+      <c r="B221" t="s">
+        <v>22</v>
+      </c>
+      <c r="C221" t="s">
+        <v>44</v>
+      </c>
+      <c r="D221">
+        <v>70</v>
+      </c>
+      <c r="E221" t="s">
+        <v>19</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G221">
+        <v>384</v>
+      </c>
+      <c r="H221" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>348</v>
+      </c>
+      <c r="B222" t="s">
+        <v>22</v>
+      </c>
+      <c r="C222" t="s">
+        <v>44</v>
+      </c>
+      <c r="D222">
+        <v>41</v>
+      </c>
+      <c r="E222" t="s">
+        <v>14</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G222">
+        <v>384</v>
+      </c>
+      <c r="H222" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>348</v>
+      </c>
+      <c r="B223" t="s">
+        <v>22</v>
+      </c>
+      <c r="C223" t="s">
+        <v>44</v>
+      </c>
+      <c r="D223">
+        <v>42</v>
+      </c>
+      <c r="E223" t="s">
+        <v>18</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G223">
+        <v>384</v>
+      </c>
+      <c r="H223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>348</v>
+      </c>
+      <c r="B224" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224" t="s">
+        <v>44</v>
+      </c>
+      <c r="D224">
+        <v>43</v>
+      </c>
+      <c r="E224" t="s">
+        <v>19</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G224">
+        <v>384</v>
+      </c>
+      <c r="H224" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>348</v>
+      </c>
+      <c r="B225" t="s">
+        <v>22</v>
+      </c>
+      <c r="C225" t="s">
+        <v>44</v>
+      </c>
+      <c r="D225">
+        <v>44</v>
+      </c>
+      <c r="E225" t="s">
+        <v>14</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G225">
+        <v>384</v>
+      </c>
+      <c r="H225" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>348</v>
+      </c>
+      <c r="B226" t="s">
+        <v>22</v>
+      </c>
+      <c r="C226" t="s">
+        <v>44</v>
+      </c>
+      <c r="D226">
+        <v>45</v>
+      </c>
+      <c r="E226" t="s">
+        <v>18</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G226">
+        <v>384</v>
+      </c>
+      <c r="H226" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>348</v>
+      </c>
+      <c r="B227" t="s">
+        <v>22</v>
+      </c>
+      <c r="C227" t="s">
+        <v>44</v>
+      </c>
+      <c r="D227">
+        <v>46</v>
+      </c>
+      <c r="E227" t="s">
+        <v>19</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G227">
+        <v>384</v>
+      </c>
+      <c r="H227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>348</v>
+      </c>
+      <c r="B228" t="s">
+        <v>22</v>
+      </c>
+      <c r="C228" t="s">
+        <v>44</v>
+      </c>
+      <c r="D228">
+        <v>47</v>
+      </c>
+      <c r="E228" t="s">
+        <v>14</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G228">
+        <v>384</v>
+      </c>
+      <c r="H228" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>348</v>
+      </c>
+      <c r="B229" t="s">
+        <v>22</v>
+      </c>
+      <c r="C229" t="s">
+        <v>44</v>
+      </c>
+      <c r="D229">
+        <v>48</v>
+      </c>
+      <c r="E229" t="s">
+        <v>18</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G229">
+        <v>384</v>
+      </c>
+      <c r="H229" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>348</v>
+      </c>
+      <c r="B230" t="s">
+        <v>22</v>
+      </c>
+      <c r="C230" t="s">
+        <v>44</v>
+      </c>
+      <c r="D230">
+        <v>49</v>
+      </c>
+      <c r="E230" t="s">
+        <v>19</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G230">
+        <v>384</v>
+      </c>
+      <c r="H230" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>348</v>
+      </c>
+      <c r="B231" t="s">
+        <v>22</v>
+      </c>
+      <c r="C231" t="s">
+        <v>44</v>
+      </c>
+      <c r="D231">
+        <v>50</v>
+      </c>
+      <c r="E231" t="s">
+        <v>14</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G231">
+        <v>384</v>
+      </c>
+      <c r="H231" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>348</v>
+      </c>
+      <c r="B232" t="s">
+        <v>22</v>
+      </c>
+      <c r="C232" t="s">
+        <v>44</v>
+      </c>
+      <c r="D232">
+        <v>51</v>
+      </c>
+      <c r="E232" t="s">
+        <v>18</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G232">
+        <v>384</v>
+      </c>
+      <c r="H232" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>348</v>
+      </c>
+      <c r="B233" t="s">
+        <v>22</v>
+      </c>
+      <c r="C233" t="s">
+        <v>44</v>
+      </c>
+      <c r="D233">
+        <v>52</v>
+      </c>
+      <c r="E233" t="s">
+        <v>19</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G233">
+        <v>384</v>
+      </c>
+      <c r="H233" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>348</v>
+      </c>
+      <c r="B234" t="s">
+        <v>22</v>
+      </c>
+      <c r="C234" t="s">
+        <v>44</v>
+      </c>
+      <c r="D234">
+        <v>53</v>
+      </c>
+      <c r="E234" t="s">
+        <v>14</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G234">
+        <v>384</v>
+      </c>
+      <c r="H234" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>348</v>
+      </c>
+      <c r="B235" t="s">
+        <v>22</v>
+      </c>
+      <c r="C235" t="s">
+        <v>44</v>
+      </c>
+      <c r="D235">
+        <v>54</v>
+      </c>
+      <c r="E235" t="s">
+        <v>18</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G235">
+        <v>384</v>
+      </c>
+      <c r="H235" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>348</v>
+      </c>
+      <c r="B236" t="s">
+        <v>22</v>
+      </c>
+      <c r="C236" t="s">
+        <v>44</v>
+      </c>
+      <c r="D236">
+        <v>55</v>
+      </c>
+      <c r="E236" t="s">
+        <v>19</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G236">
+        <v>384</v>
+      </c>
+      <c r="H236" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>348</v>
+      </c>
+      <c r="B237" t="s">
+        <v>22</v>
+      </c>
+      <c r="C237" t="s">
+        <v>44</v>
+      </c>
+      <c r="D237">
+        <v>56</v>
+      </c>
+      <c r="E237" t="s">
+        <v>14</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G237">
+        <v>384</v>
+      </c>
+      <c r="H237" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>348</v>
+      </c>
+      <c r="B238" t="s">
+        <v>22</v>
+      </c>
+      <c r="C238" t="s">
+        <v>44</v>
+      </c>
+      <c r="D238">
+        <v>57</v>
+      </c>
+      <c r="E238" t="s">
+        <v>18</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G238">
+        <v>384</v>
+      </c>
+      <c r="H238" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>348</v>
+      </c>
+      <c r="B239" t="s">
+        <v>22</v>
+      </c>
+      <c r="C239" t="s">
+        <v>44</v>
+      </c>
+      <c r="D239">
+        <v>58</v>
+      </c>
+      <c r="E239" t="s">
+        <v>19</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G239">
+        <v>384</v>
+      </c>
+      <c r="H239" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>348</v>
+      </c>
+      <c r="B240" t="s">
+        <v>22</v>
+      </c>
+      <c r="C240" t="s">
+        <v>44</v>
+      </c>
+      <c r="D240">
+        <v>59</v>
+      </c>
+      <c r="E240" t="s">
+        <v>14</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G240">
+        <v>384</v>
+      </c>
+      <c r="H240" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>348</v>
+      </c>
+      <c r="B241" t="s">
+        <v>22</v>
+      </c>
+      <c r="C241" t="s">
+        <v>44</v>
+      </c>
+      <c r="D241">
+        <v>60</v>
+      </c>
+      <c r="E241" t="s">
+        <v>18</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G241">
+        <v>384</v>
+      </c>
+      <c r="H241" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>348</v>
+      </c>
+      <c r="B242" t="s">
+        <v>22</v>
+      </c>
+      <c r="C242" t="s">
+        <v>44</v>
+      </c>
+      <c r="D242">
+        <v>61</v>
+      </c>
+      <c r="E242" t="s">
+        <v>19</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G242">
+        <v>384</v>
+      </c>
+      <c r="H242" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>348</v>
+      </c>
+      <c r="B243" t="s">
+        <v>22</v>
+      </c>
+      <c r="C243" t="s">
+        <v>44</v>
+      </c>
+      <c r="D243">
+        <v>62</v>
+      </c>
+      <c r="E243" t="s">
+        <v>14</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G243">
+        <v>384</v>
+      </c>
+      <c r="H243" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>348</v>
+      </c>
+      <c r="B244" t="s">
+        <v>22</v>
+      </c>
+      <c r="C244" t="s">
+        <v>44</v>
+      </c>
+      <c r="D244">
+        <v>63</v>
+      </c>
+      <c r="E244" t="s">
+        <v>18</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G244">
+        <v>384</v>
+      </c>
+      <c r="H244" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>348</v>
+      </c>
+      <c r="B245" t="s">
+        <v>22</v>
+      </c>
+      <c r="C245" t="s">
+        <v>44</v>
+      </c>
+      <c r="D245">
+        <v>64</v>
+      </c>
+      <c r="E245" t="s">
+        <v>19</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G245">
+        <v>384</v>
+      </c>
+      <c r="H245" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>348</v>
+      </c>
+      <c r="B246" t="s">
+        <v>22</v>
+      </c>
+      <c r="C246" t="s">
+        <v>44</v>
+      </c>
+      <c r="D246">
+        <v>65</v>
+      </c>
+      <c r="E246" t="s">
+        <v>14</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G246">
+        <v>384</v>
+      </c>
+      <c r="H246" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>348</v>
+      </c>
+      <c r="B247" t="s">
+        <v>22</v>
+      </c>
+      <c r="C247" t="s">
+        <v>44</v>
+      </c>
+      <c r="D247">
+        <v>66</v>
+      </c>
+      <c r="E247" t="s">
+        <v>18</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G247">
+        <v>384</v>
+      </c>
+      <c r="H247" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>348</v>
+      </c>
+      <c r="B248" t="s">
+        <v>22</v>
+      </c>
+      <c r="C248" t="s">
+        <v>44</v>
+      </c>
+      <c r="D248">
+        <v>67</v>
+      </c>
+      <c r="E248" t="s">
+        <v>19</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G248">
+        <v>384</v>
+      </c>
+      <c r="H248" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>348</v>
+      </c>
+      <c r="B249" t="s">
+        <v>22</v>
+      </c>
+      <c r="C249" t="s">
+        <v>44</v>
+      </c>
+      <c r="D249">
+        <v>68</v>
+      </c>
+      <c r="E249" t="s">
+        <v>14</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G249">
+        <v>384</v>
+      </c>
+      <c r="H249" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>348</v>
+      </c>
+      <c r="B250" t="s">
+        <v>22</v>
+      </c>
+      <c r="C250" t="s">
+        <v>44</v>
+      </c>
+      <c r="D250">
+        <v>69</v>
+      </c>
+      <c r="E250" t="s">
+        <v>18</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G250">
+        <v>384</v>
+      </c>
+      <c r="H250" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>348</v>
+      </c>
+      <c r="B251" t="s">
+        <v>22</v>
+      </c>
+      <c r="C251" t="s">
+        <v>44</v>
+      </c>
+      <c r="D251">
+        <v>70</v>
+      </c>
+      <c r="E251" t="s">
+        <v>19</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G251">
+        <v>384</v>
+      </c>
+      <c r="H251" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>351</v>
+      </c>
+      <c r="B252" t="s">
+        <v>22</v>
+      </c>
+      <c r="C252" t="s">
+        <v>45</v>
+      </c>
+      <c r="D252">
+        <v>121</v>
+      </c>
+      <c r="E252" t="s">
+        <v>14</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G252">
+        <v>384</v>
+      </c>
+      <c r="H252" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>351</v>
+      </c>
+      <c r="B253" t="s">
+        <v>22</v>
+      </c>
+      <c r="C253" t="s">
+        <v>45</v>
+      </c>
+      <c r="D253">
+        <v>122</v>
+      </c>
+      <c r="E253" t="s">
+        <v>18</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G253">
+        <v>384</v>
+      </c>
+      <c r="H253" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>351</v>
+      </c>
+      <c r="B254" t="s">
+        <v>22</v>
+      </c>
+      <c r="C254" t="s">
+        <v>45</v>
+      </c>
+      <c r="D254">
+        <v>123</v>
+      </c>
+      <c r="E254" t="s">
+        <v>19</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G254">
+        <v>384</v>
+      </c>
+      <c r="H254" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>351</v>
+      </c>
+      <c r="B255" t="s">
+        <v>22</v>
+      </c>
+      <c r="C255" t="s">
+        <v>45</v>
+      </c>
+      <c r="D255">
+        <v>124</v>
+      </c>
+      <c r="E255" t="s">
+        <v>14</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G255">
+        <v>384</v>
+      </c>
+      <c r="H255" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>351</v>
+      </c>
+      <c r="B256" t="s">
+        <v>22</v>
+      </c>
+      <c r="C256" t="s">
+        <v>45</v>
+      </c>
+      <c r="D256">
+        <v>125</v>
+      </c>
+      <c r="E256" t="s">
+        <v>18</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G256">
+        <v>384</v>
+      </c>
+      <c r="H256" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>351</v>
+      </c>
+      <c r="B257" t="s">
+        <v>22</v>
+      </c>
+      <c r="C257" t="s">
+        <v>45</v>
+      </c>
+      <c r="D257">
+        <v>126</v>
+      </c>
+      <c r="E257" t="s">
+        <v>19</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G257">
+        <v>384</v>
+      </c>
+      <c r="H257" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>351</v>
+      </c>
+      <c r="B258" t="s">
+        <v>22</v>
+      </c>
+      <c r="C258" t="s">
+        <v>45</v>
+      </c>
+      <c r="D258">
+        <v>127</v>
+      </c>
+      <c r="E258" t="s">
+        <v>14</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G258">
+        <v>384</v>
+      </c>
+      <c r="H258" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>351</v>
+      </c>
+      <c r="B259" t="s">
+        <v>22</v>
+      </c>
+      <c r="C259" t="s">
+        <v>45</v>
+      </c>
+      <c r="D259">
+        <v>128</v>
+      </c>
+      <c r="E259" t="s">
+        <v>18</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G259">
+        <v>384</v>
+      </c>
+      <c r="H259" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>351</v>
+      </c>
+      <c r="B260" t="s">
+        <v>22</v>
+      </c>
+      <c r="C260" t="s">
+        <v>45</v>
+      </c>
+      <c r="D260">
+        <v>129</v>
+      </c>
+      <c r="E260" t="s">
+        <v>19</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G260">
+        <v>384</v>
+      </c>
+      <c r="H260" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>351</v>
+      </c>
+      <c r="B261" t="s">
+        <v>22</v>
+      </c>
+      <c r="C261" t="s">
+        <v>45</v>
+      </c>
+      <c r="D261">
+        <v>130</v>
+      </c>
+      <c r="E261" t="s">
+        <v>14</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G261">
+        <v>384</v>
+      </c>
+      <c r="H261" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>351</v>
+      </c>
+      <c r="B262" t="s">
+        <v>22</v>
+      </c>
+      <c r="C262" t="s">
+        <v>45</v>
+      </c>
+      <c r="D262">
+        <v>131</v>
+      </c>
+      <c r="E262" t="s">
+        <v>18</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G262">
+        <v>384</v>
+      </c>
+      <c r="H262" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>351</v>
+      </c>
+      <c r="B263" t="s">
+        <v>22</v>
+      </c>
+      <c r="C263" t="s">
+        <v>45</v>
+      </c>
+      <c r="D263">
+        <v>132</v>
+      </c>
+      <c r="E263" t="s">
+        <v>19</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G263">
+        <v>384</v>
+      </c>
+      <c r="H263" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>352</v>
+      </c>
+      <c r="B264" t="s">
+        <v>22</v>
+      </c>
+      <c r="C264" t="s">
+        <v>47</v>
+      </c>
+      <c r="D264">
+        <v>141</v>
+      </c>
+      <c r="E264" t="s">
+        <v>46</v>
+      </c>
+      <c r="F264" t="s">
+        <v>31</v>
+      </c>
+      <c r="G264">
+        <v>384</v>
+      </c>
+      <c r="H264" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>352</v>
+      </c>
+      <c r="B265" t="s">
+        <v>22</v>
+      </c>
+      <c r="C265" t="s">
+        <v>47</v>
+      </c>
+      <c r="D265">
+        <v>142</v>
+      </c>
+      <c r="E265" t="s">
+        <v>46</v>
+      </c>
+      <c r="F265" t="s">
+        <v>48</v>
+      </c>
+      <c r="G265">
+        <v>384</v>
+      </c>
+      <c r="H265" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>352</v>
+      </c>
+      <c r="B266" t="s">
+        <v>22</v>
+      </c>
+      <c r="C266" t="s">
+        <v>47</v>
+      </c>
+      <c r="D266">
+        <v>143</v>
+      </c>
+      <c r="E266" t="s">
+        <v>46</v>
+      </c>
+      <c r="F266" t="s">
+        <v>31</v>
+      </c>
+      <c r="G266">
+        <v>384</v>
+      </c>
+      <c r="H266" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>352</v>
+      </c>
+      <c r="B267" t="s">
+        <v>22</v>
+      </c>
+      <c r="C267" t="s">
+        <v>47</v>
+      </c>
+      <c r="D267">
+        <v>144</v>
+      </c>
+      <c r="E267" t="s">
+        <v>46</v>
+      </c>
+      <c r="F267" t="s">
+        <v>48</v>
+      </c>
+      <c r="G267">
+        <v>384</v>
+      </c>
+      <c r="H267" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>352</v>
+      </c>
+      <c r="B268" t="s">
+        <v>22</v>
+      </c>
+      <c r="C268" t="s">
+        <v>47</v>
+      </c>
+      <c r="D268">
+        <v>145</v>
+      </c>
+      <c r="E268" t="s">
+        <v>46</v>
+      </c>
+      <c r="F268" t="s">
+        <v>31</v>
+      </c>
+      <c r="G268">
+        <v>384</v>
+      </c>
+      <c r="H268" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>352</v>
+      </c>
+      <c r="B269" t="s">
+        <v>22</v>
+      </c>
+      <c r="C269" t="s">
+        <v>47</v>
+      </c>
+      <c r="D269">
+        <v>146</v>
+      </c>
+      <c r="E269" t="s">
+        <v>46</v>
+      </c>
+      <c r="F269" t="s">
+        <v>48</v>
+      </c>
+      <c r="G269">
+        <v>384</v>
+      </c>
+      <c r="H269" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>